<commit_message>
Updated status of SSO risk.
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -19,7 +19,326 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
+  <si>
+    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.
+This is a major undertaking, and will have to be deferred until after release v1.4. The team has shifted focus to bug fixes.
+Note that there is no major impact to the user:
+* Single Sign-on still works for the major use case - a user can navigate between the caIntegrator and caArray web applications without having to type in credentials again. This is 90% of the use case.
+* The only place where the user cannot take advantage of SSO is when a caIntegrator Study Manager first sets up a study and adds a genomic data source. He/she will have to type in their credentials at this point, similar to how it works today.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the issue is not resolved by the end of June 8, a strategy would be to release with Single Sign-on working in only the web application layer (linking to a caArray experiment from caIntegrator, and navigating between the 2 applications in a web browser).</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coordinated release of caArray, caIntegrator and UPT is needed for tech stack consistency.</t>
+  </si>
+  <si>
+    <t>Rashmi and Shine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The dependencies among teams is a risk to the schedule of each individual project.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The caArray and caIntegrator project plans were adjusted to account for these priorities, and project plan walthroughs were completed in January 2012.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retirement of old Ivy and Gforge repositories will result in users being unable to build from source code of older versions of caArray and caIntegrator.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>After evaluation and final solution of the data load problem, the schedule for caArray releases has been moved out to accommodate this extra requirement.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAS set-up on the Dev tier is done and testing is ongoing. QA tier has not been set up yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old tech stack in caIntegrator prevents EJB-layer SSO from working</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Significant maintenance and engineering work affect feature development in SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline and support from Systems team.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New CIT policy re: Medium vulnerabilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Developer for caIntegrator coming on board late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>An experienced caBIG developer is on board October 1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BDA-Lite requirements adds to scope</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nobody</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments/Resolution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impact</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Risk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mitigation Plan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSCEND architecture decisions will affect scope significantly</t>
+  </si>
+  <si>
+    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No support for BDA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Release coordination with API partners</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -139,289 +458,6 @@
     <t>We will go ahead with testing of I-SPY1 data, but once
 the I-SPY2 data is available, we would like to test with those as
 well.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No support for BDA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAS set-up on the Dev tier is expected in the first week of May.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Significant maintenance and engineering work affect feature development in SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline and support from Systems team.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>New CIT policy re: Medium vulnerabilities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Developer for caIntegrator coming on board late</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>An experienced caBIG developer is on board October 1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BDA-Lite requirements adds to scope</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nobody</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comments/Resolution</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Impact</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Risk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mitigation Plan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSCEND architecture decisions will affect scope significantly</t>
-  </si>
-  <si>
-    <t>Coordinated release of caArray, caIntegrator and UPT is needed for tech stack consistency.</t>
-  </si>
-  <si>
-    <t>Rashmi and Shine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The dependencies among teams is a risk to the schedule of each individual project.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The caArray and caIntegrator project plans were adjusted to account for these priorities, and project plan walthroughs were completed in January 2012.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retirement of old Ivy and Gforge repositories will result in users being unable to build from source code of older versions of caArray and caIntegrator.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>After evaluation and final solution of the data load problem, the schedule for caArray releases has been moved out to accommodate this extra requirement.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -429,12 +465,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -837,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -859,454 +889,483 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="39">
       <c r="A2" s="6" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="52">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A6" s="6" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A7" s="6" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A9" s="6" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="H9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="39">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="26">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A15" s="6" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39">
       <c r="A16" s="3" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="52">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="182">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1374,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated CAS and API risks.
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -21,6 +21,379 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
   <si>
+    <t>The caArray 2.4.1 source code has been patched to work with the new NCI repositories.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>Availability of sample data files of all types from I-SPY2 for loading into caArray and testing</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>Availability of CAS set up on Dev, QA and STAGE tiers for Single Sign-on testing</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Availability of UCSF personnel for UAT</t>
+  </si>
+  <si>
+    <t>Rashmi and Shine</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>We will go ahead with testing of I-SPY1 data, but once
+the I-SPY2 data is available, we would like to test with those as
+well.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rembrandt is testing now. As of June 12, GenePattern does not have the time to test yet, and caB2B has not started testing either.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAS set-up on the Dev tier is done and testing is ongoing. QA tier has not been set up yet. Latest from Cuong is that the server will be delivered some time between June 15 and June 22, and then the Systems team will have to configure it after that.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release coordination with API partners</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All of caArray's API partners have to upgrade their client jars in order to work with the new caArray 2.5.0. This means that their release schedules need to be coordinated with caArray's.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release caArray 2.5.0 for local installers in July, but don't upgrade the NCI Production caArray tier to 2.5.0 until partners are ready in August.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">caIntegrator and caArray tech stack upgrades will not be completed until the new UPT release is available. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Availability of new UPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource shortage has affected schedule</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unexpected leaving of developers affected velocity temporarily, but new developers have caught us up.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overloading of QA team</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy is overloaded with multiple projects to test, and is not able to devote sufficient time to test caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release without adequate QA testing.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy is responsible for testing all caArray featues including the ones for TRANSCEND. His availability is crucial to be able to deliver a quality product.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nobody</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments/Resolution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impact</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Risk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mitigation Plan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSCEND architecture decisions will affect scope significantly</t>
+  </si>
+  <si>
+    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No support for BDA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old tech stack in caIntegrator prevents EJB-layer SSO from working</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Significant maintenance and engineering work affect feature development in SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline and support from Systems team.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New CIT policy re: Medium vulnerabilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Developer for caIntegrator coming on board late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>An experienced caBIG developer is on board October 1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BDA-Lite requirements adds to scope</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.
 This is a major undertaking, and will have to be deferred until after release v1.4. The team has shifted focus to bug fixes.
 Note that there is no major impact to the user:
@@ -85,379 +458,6 @@
   </si>
   <si>
     <t>After evaluation and final solution of the data load problem, the schedule for caArray releases has been moved out to accommodate this extra requirement.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAS set-up on the Dev tier is done and testing is ongoing. QA tier has not been set up yet.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R17</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old tech stack in caIntegrator prevents EJB-layer SSO from working</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Significant maintenance and engineering work affect feature development in SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline and support from Systems team.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>New CIT policy re: Medium vulnerabilities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Developer for caIntegrator coming on board late</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>An experienced caBIG developer is on board October 1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BDA-Lite requirements adds to scope</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nobody</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comments/Resolution</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Impact</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Risk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mitigation Plan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSCEND architecture decisions will affect scope significantly</t>
-  </si>
-  <si>
-    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No support for BDA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release coordination with API partners</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>All of caArray's API partners have to upgrade their client jars in order to work with the new caArray 2.5.0. This means that their release schedules need to be coordinated with caArray's.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release caArray 2.5.0 for local installers in July, but don't upgrade the NCI Production caArray tier to 2.5.0 until partners are ready in August.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rembrandt seems to be the only application of concern.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">caIntegrator and caArray tech stack upgrades will not be completed until the new UPT release is available. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R13</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R14</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R15</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Availability of new UPT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resource shortage has affected schedule</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unexpected leaving of developers affected velocity temporarily, but new developers have caught us up.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overloading of QA team</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy is overloaded with multiple projects to test, and is not able to devote sufficient time to test caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release without adequate QA testing.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy is responsible for testing all caArray featues including the ones for TRANSCEND. His availability is crucial to be able to deliver a quality product.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The caArray 2.4.1 source code has been patched to work with the new NCI repositories.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>Availability of sample data files of all types from I-SPY2 for loading into caArray and testing</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>Availability of CAS set up on Dev, QA and STAGE tiers for Single Sign-on testing</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Availability of UCSF personnel for UAT</t>
-  </si>
-  <si>
-    <t>Rashmi and Shine</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>We will go ahead with testing of I-SPY1 data, but once
-the I-SPY2 data is available, we would like to test with those as
-well.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -889,483 +889,483 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="39">
       <c r="A2" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="52">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="I5" s="7" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A9" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39">
       <c r="A11" s="3" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="5" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="52">
       <c r="A12" s="3" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="26">
       <c r="A14" s="3" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="52">
       <c r="A17" s="3" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="182">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest status of risks.
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -19,7 +19,380 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="114">
+  <si>
+    <t>Quy is responsible for testing all caArray features including the ones for TRANSCEND. Hisfull-time availability is crucial to be able to deliver a quality product.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">caIntegrator and caArray have completed this upgrade. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>As of June 12, GenePattern does not have the time to test yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release coordination with API partners</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All of caArray's API partners have to upgrade their client jars in order to work with the new caArray 2.5.0. This means that their release schedules need to be coordinated with caArray's.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAS and SSO set-up on the NCI Dev and QA tiers - Troubleshooting of AHP build workflow problems is done now, but it was completed after tagging the first release candidate RC1. This does not give us enough opportunity to test in SSO mode on the NCI tiers, but we have tested on local installations instead.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We have provided 3 drops to UCSF for UAT, but they have not had the time to test and provide feedback yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release without adequate QA testing.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nobody</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments/Resolution</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Impact</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Risk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mitigation Plan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSCEND architecture decisions will affect scope significantly</t>
+  </si>
+  <si>
+    <t>The caArray 2.4.1 source code has been patched to work with the new NCI repositories.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>Availability of sample data files of all types from I-SPY2 for loading into caArray and testing</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>Availability of CAS set up on Dev, QA and STAGE tiers for Single Sign-on testing</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Availability of UCSF personnel for UAT</t>
+  </si>
+  <si>
+    <t>Rashmi and Shine</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Eve Shalley</t>
+  </si>
+  <si>
+    <t>We will go ahead with testing of I-SPY1 data, but once
+the I-SPY2 data is available, we would like to test with those as
+well.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No support for BDA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old tech stack in caIntegrator prevents EJB-layer SSO from working</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Significant maintenance and engineering work affect feature development in SOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Juli Klemm and Mervi Heiskanen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Release caArray 2.5.0 for local installers in July, but don't upgrade the NCI Production caArray tier to 2.5.0 until partners are ready in August.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Availability of new UPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shine and Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource shortage has affected schedule</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rashmi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unexpected leaving of developers affected velocity temporarily, but new developers have caught us up.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overloading of QA team</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quy is overloaded with multiple projects to test, and is not able to devote sufficient time to test caArray.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discuss timeline and support from Systems team.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New CIT policy re: Medium vulnerabilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
+  </si>
+  <si>
+    <t>Rashmi Srinivasa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Developer for caIntegrator coming on board late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>An experienced caBIG developer is on board October 1.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BDA-Lite requirements adds to scope</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.
 This is a major undertaking, and has been deferred until after release v1.4. The team has shifted focus to bug fixes.
@@ -37,10 +410,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">caIntegrator and caArray have complete this upgrade. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>If the issue is not resolved by the end of June 8, a strategy would be to release with Single Sign-on working in only the web application layer (linking to a caArray experiment from caIntegrator, and navigating between the 2 applications in a web browser).</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -97,371 +466,6 @@
   </si>
   <si>
     <t>After evaluation and final solution of the data load problem, the schedule for caArray releases has been moved out to accommodate this extra requirement.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>As of June 12, GenePattern does not have the time to test yet.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline and support from Systems team.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>New CIT policy re: Medium vulnerabilities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The new CIT security policy of mandating resolution of Medium vulnerabilities from app scans will impact the schedule of upcoming releases for caArray and caIntegrator.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Short-term solution for the TCGA large data set support was added late to the caArray scope.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The short-term solution to the TCGA data load problem was added late and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The second developer for caIntegrator will come on board on October 1 instead of on September 1, 2011</t>
-  </si>
-  <si>
-    <t>Rashmi Srinivasa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Developer for caIntegrator coming on board late</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The risk has been communicated to the NCI, and the current decision is to continue with the reliance on the patched BDA code.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>An experienced caBIG developer is on board October 1.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BDA-Lite requirements adds to scope</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The TRANSCEND architecture has been finalized and the project plan has been updated.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Many applications (including caArray and caIntegrator) rely on the BDA jars to do build, deploy and artifact-generation/configuration (e.g., installers/upgraders). With the move to BDALite, several build modifications have been made, and the BDA code has been patched to work with the new NCI/Nexus repositories. However, there is a risk remaining in that these applications still depend on the patched BDA code, and there is no team at the NCI to support that code any more. The best solution would be to rewrite the build and deploy scripts for these applications from scratch, removing all reliance on the BDA code, but this will be time-consuming.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The current release under development (e.g., caArray 2.5.0) has been updated (along with the BDA version it uses - 1.7) to refer to the new repositories. However, older versions (e.g., caArray 2.4.1, 2.4.0. 2.3.1.1, etc.) have not been upgraded in this way. This means that if a user tries to build these older versions from source code, the build will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan, Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ask the Systems team to resurrect the old Ivy/Gforge repositories in a read-only mode for a few months.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No support for BDA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The schedule has been extended to accommodate these extra requirements. BDALite has now been implemented on the DEV, QA and STAGE tiers, but not on PRODUCTION yet.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R17</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old tech stack in caIntegrator prevents EJB-layer SSO from working</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caIntegrator uses Acegi security, and this feature seems to require an upgrade of the security framework to Spring security.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Significant maintenance and engineering work affect feature development in SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prioritize requirements with Juli, Mervi and JJ.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Juli Klemm and Mervi Heiskanen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release caArray 2.5.0 for local installers in July, but don't upgrade the NCI Production caArray tier to 2.5.0 until partners are ready in August.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R13</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R14</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R15</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R16</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Availability of new UPT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shine and Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resource shortage has affected schedule</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rashmi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unexpected leaving of developers affected velocity temporarily, but new developers have caught us up.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overloading of QA team</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy is overloaded with multiple projects to test, and is not able to devote sufficient time to test caArray.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release without adequate QA testing.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quy is responsible for testing all caArray featues including the ones for TRANSCEND. His availability is crucial to be able to deliver a quality product.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The enterprise-mandated BDA-Lite requirement has added to the scope of both caArray and caIntegrator and has impacted the schedule.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JJ Pan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nobody</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comments/Resolution</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Impact</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Risk</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mitigation Plan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TRANSCEND architecture decisions will affect scope significantly</t>
-  </si>
-  <si>
-    <t>The caArray 2.4.1 source code has been patched to work with the new NCI repositories.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>Availability of sample data files of all types from I-SPY2 for loading into caArray and testing</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>Availability of CAS set up on Dev, QA and STAGE tiers for Single Sign-on testing</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Availability of UCSF personnel for UAT</t>
-  </si>
-  <si>
-    <t>Rashmi and Shine</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Eve Shalley</t>
-  </si>
-  <si>
-    <t>We will go ahead with testing of I-SPY1 data, but once
-the I-SPY2 data is available, we would like to test with those as
-well.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAS set-up on the Dev tier is done and testing is ongoing. QA tier has not been set up yet. Latest from Cuong is that the server will be delivered some time between June 15 and June 22, and then the Systems team will have to configure it after that.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Both the caArray and caIntegrator teams are putting a significant amount of effort towards maintenance and engineering activities (like 508 compliance, security issues, tech stack upgrades) now. These are important activities, but they were not listed specifically and may have an impact on the deliverables for the other features listed on SOW</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>High</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discuss timeline from Systems team. Schedule early preparatory app scans to discover problems earlier.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray 2.4.1 and caIntegrator 1.3 addressed these new requirements and were successfully released.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Release coordination with API partners</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>All of caArray's API partners have to upgrade their client jars in order to work with the new caArray 2.5.0. This means that their release schedules need to be coordinated with caArray's.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -469,6 +473,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -873,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -893,484 +903,486 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="39">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="52">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="91">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="I7" s="7" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="156">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A9" s="6" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="5" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="52">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="65">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="26">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="6" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" ht="26">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39">
       <c r="A16" s="3" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="52">
       <c r="A17" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="6" customFormat="1" ht="182">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1379,6 +1391,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated agenda, project plan, action items and risks.
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
   <si>
     <t>Medium</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>Budget limitations have reduced the team size to half a developer for each of the two applications, and progress is slow. Effective resolution of issues requires a bigger team size.</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>Updating AHP builds is on hold due to ongoing discussions among Juli, JJ and Doug Hosier about Systems team support. This is a risk since future code changes will happen on GitHub and we will not be able to test on the Dev/QA tiers. (The QA team is scheduled to start regression testing the next release on the QA tier on March 12.)</t>
+  </si>
+  <si>
+    <t>Juli, JJ and Doug Hosier</t>
+  </si>
+  <si>
+    <t>After OSDI migration to GitHub, code cannot be tested on NCI tiers due to the AntHill Pro updates being on hold</t>
   </si>
 </sst>
 </file>
@@ -326,8 +338,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -356,17 +370,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -694,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -919,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>0</v>
@@ -950,22 +966,22 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="30">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1087,24 +1103,44 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90">
+      <c r="A21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>75</v>
+      <c r="F21" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for 4/16 status meeting
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>Medium</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>After OSDI migration to GitHub, code cannot be tested on NCI tiers due to the AntHill Pro updates being on hold</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>Transition from Rashmi to Mike Hunter will result in loss of historical knowledge and project context</t>
+  </si>
+  <si>
+    <t>Ulli, Juli and JJ</t>
+  </si>
+  <si>
+    <t>5AM submitted a training plan for Mike's first two months to mitigate the impact of Rashmi leaving the project.  The plan was accepted and is underway.  Mike also has access to Will Fitzhugh and Todd Parnell as a recourse if significant issues arise.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +312,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +322,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +356,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -352,8 +370,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -369,20 +389,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1124,23 +1149,43 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="90">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75">
+      <c r="A22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>77</v>
+      <c r="F22" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
End of month status updates
</commit_message>
<xml_diff>
--- a/project_management/caArray_Risks.xlsx
+++ b/project_management/caArray_Risks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="2100" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Risks" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>Medium</t>
   </si>
@@ -275,6 +275,30 @@
   </si>
   <si>
     <t>5AM submitted a training plan for Mike's first two months to mitigate the impact of Rashmi leaving the project.  The plan was accepted and is underway.  Mike also has access to Will Fitzhugh and Todd Parnell as a recourse if significant issues arise.</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>QA will be handled by Ji while Marina is out from 7/1 to 7/18.   This may slow the process of getting caArray and caIntegrator approved to go to the DEMO/STAGING tier, if we don't get approval before 7/1.</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We're entering the period when people take vacations.  This may slow communication and impact the pace of work.</t>
+  </si>
+  <si>
+    <t>Mike Hunter</t>
+  </si>
+  <si>
+    <t>Mike will follow up with team members to find out when they plan to be out and confirm that each team member has identified an appropriate backup to represent them in making decisions or otherwise cover their work while they are away.</t>
+  </si>
+  <si>
+    <t>With caArray 2.5.1 we're going through a new SOP for promotion to DEMO/STAGING tier with new team members (Marina, Mike), so we should expect some initial misses and confusion while we learn the SOP.  This may slow the process of getting approval.</t>
   </si>
 </sst>
 </file>
@@ -373,7 +397,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,6 +415,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -735,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1188,6 +1216,58 @@
         <v>83</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="90">
+      <c r="A23" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="60">
+      <c r="A24" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="105">
+      <c r="A25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
   </sheetData>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="A3:A1048576"/>

</xml_diff>